<commit_message>
LongNH update: - build base code Router - update Document
</commit_message>
<xml_diff>
--- a/documents/API Design.xlsx
+++ b/documents/API Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyenhoanglong\Desktop\facebook-api-system\facebook-api-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B30663-A75F-4361-BF35-0EE4E6DF64D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1D36EC-A973-494D-8D45-B1EB5A03BADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9981A1F3-371F-4819-8FA9-3C3705423757}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9981A1F3-371F-4819-8FA9-3C3705423757}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -126,21 +126,6 @@
     <t>homePage</t>
   </si>
   <si>
-    <t>/user/saveProfile</t>
-  </si>
-  <si>
-    <t>/user/postStatus</t>
-  </si>
-  <si>
-    <t>/user/comment</t>
-  </si>
-  <si>
-    <t>/user/reactStatus</t>
-  </si>
-  <si>
-    <t>/user/addFriend</t>
-  </si>
-  <si>
     <t>/home</t>
   </si>
   <si>
@@ -166,6 +151,21 @@
   </si>
   <si>
     <t>/account/createNewPassword</t>
+  </si>
+  <si>
+    <t>/profile/saveProfile</t>
+  </si>
+  <si>
+    <t>/profile/postStatus</t>
+  </si>
+  <si>
+    <t>/profile/comment</t>
+  </si>
+  <si>
+    <t>/profile/reactStatus</t>
+  </si>
+  <si>
+    <t>/profile/addFriend</t>
   </si>
 </sst>
 </file>
@@ -245,9 +245,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -269,6 +266,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -587,15 +587,15 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="20.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="20.140625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="34.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="25.42578125" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
@@ -605,51 +605,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3" t="s">
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="1:13" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
       <c r="G2" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -657,273 +657,273 @@
       <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
-      <c r="L3" s="9"/>
-      <c r="M3" s="9"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="7">
-        <v>2</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="9" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F9" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="9"/>
+      <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="M5" s="9"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="7">
-        <v>3</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="9" t="s">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" s="9" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="9"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
-        <v>4</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="9" t="s">
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+    </row>
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
-        <v>5</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
-        <v>6</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>7</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>8</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-    </row>
-    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>9</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
commit: init code for forgotPassword
</commit_message>
<xml_diff>
--- a/documents/API Design.xlsx
+++ b/documents/API Design.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguyenhoanglong\Desktop\facebook-api-system\facebook-api-system\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1D36EC-A973-494D-8D45-B1EB5A03BADB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51F6E4B-99DD-433F-A312-6F2B78A1C0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9981A1F3-371F-4819-8FA9-3C3705423757}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
   <si>
     <t>API Name</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>GET</t>
-  </si>
-  <si>
-    <t>GET ?</t>
   </si>
   <si>
     <t>POST ?</t>
@@ -587,7 +584,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,13 +640,13 @@
       <c r="E2" s="11"/>
       <c r="F2" s="11"/>
       <c r="G2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -671,7 +668,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
@@ -696,7 +693,7 @@
         <v>7</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
@@ -719,7 +716,7 @@
         <v>7</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
@@ -741,10 +738,10 @@
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="8" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -762,10 +759,10 @@
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -780,17 +777,17 @@
         <v>4</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -805,17 +802,17 @@
         <v>5</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -830,17 +827,17 @@
         <v>6</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -855,17 +852,17 @@
         <v>7</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>27</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -880,15 +877,15 @@
         <v>8</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -903,19 +900,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>30</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>31</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>

</xml_diff>